<commit_message>
edited the yahoo price information retrieval methods. It was returning the close price from two days. Now it uses the last trade price as the close from the day before
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/GILD/GILDpriceInformation.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/GILD/GILDpriceInformation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F5"/>
+  <dimension ref="A1:G6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -379,7 +379,7 @@
     <col min="6" max="6" width="16.28515625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -399,7 +399,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1">
         <v>42587.796412037038</v>
       </c>
@@ -419,7 +419,7 @@
         <v>-0.4</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1">
         <v>42601.774710648147</v>
       </c>
@@ -439,7 +439,7 @@
         <v>-0.14000000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1">
         <v>42601.882060185184</v>
       </c>
@@ -459,7 +459,7 @@
         <v>-0.14000000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1">
         <v>42601.883564814816</v>
       </c>
@@ -477,6 +477,29 @@
       </c>
       <c r="F5">
         <v>-0.14000000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="1">
+        <v>42601.914861111109</v>
+      </c>
+      <c r="B6" t="s">
+        <v>6</v>
+      </c>
+      <c r="C6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D6">
+        <v>80.91</v>
+      </c>
+      <c r="E6">
+        <v>80.7</v>
+      </c>
+      <c r="F6">
+        <v>-0.14000000000000001</v>
+      </c>
+      <c r="G6">
+        <v>80.59</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
wrote and tested the simulated trading section
</commit_message>
<xml_diff>
--- a/StockPredictor/bin/Debug/Packages/Data/GILD/GILDpriceInformation.xlsx
+++ b/StockPredictor/bin/Debug/Packages/Data/GILD/GILDpriceInformation.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
   <si>
     <t>Date</t>
   </si>
@@ -366,7 +366,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:G7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -502,6 +502,29 @@
         <v>80.59</v>
       </c>
     </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A7" s="1">
+        <v>42604.424884259257</v>
+      </c>
+      <c r="B7" t="s">
+        <v>6</v>
+      </c>
+      <c r="C7" t="s">
+        <v>7</v>
+      </c>
+      <c r="D7">
+        <v>80.56</v>
+      </c>
+      <c r="E7">
+        <v>81</v>
+      </c>
+      <c r="F7">
+        <v>0.51</v>
+      </c>
+      <c r="G7">
+        <v>80.59</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>